<commit_message>
Linking BOM and Schematic Template
Linking fields like 'PCBName', 'PCBDesigner', to BOM from schematic template.
</commit_message>
<xml_diff>
--- a/Shared Libraries/APSS BOM Template.xlsx
+++ b/Shared Libraries/APSS BOM Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FilipK\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vontier-my.sharepoint.com/personal/filipk_invenco_com/Documents/Documents/APSS-Reference-PCBs/Shared Libraries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9DF1E4-5EE3-4857-84AF-92CD1321BAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{BB9DF1E4-5EE3-4857-84AF-92CD1321BAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E606942-CEB7-4AF8-A26B-05FCD0F64A88}"/>
   <bookViews>
     <workbookView xWindow="1365" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{8143E680-549F-46F0-B77E-A70799F379B4}"/>
   </bookViews>
@@ -59,9 +59,6 @@
     <t>PCB Designer:</t>
   </si>
   <si>
-    <t>Field=ProjectFileName</t>
-  </si>
-  <si>
     <t>Field=ReportDate</t>
   </si>
   <si>
@@ -92,13 +89,16 @@
     <t>Column=Package</t>
   </si>
   <si>
-    <t>Field=DrawnBy</t>
-  </si>
-  <si>
-    <t>Field=Revision</t>
-  </si>
-  <si>
     <t>Field=Project</t>
+  </si>
+  <si>
+    <t>Field=PCBName</t>
+  </si>
+  <si>
+    <t>Field=PCBRevision</t>
+  </si>
+  <si>
+    <t>Field=PCBDesigner</t>
   </si>
 </sst>
 </file>
@@ -237,6 +237,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -246,7 +247,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,7 +633,7 @@
   <dimension ref="B2:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -649,36 +649,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
@@ -687,59 +687,59 @@
       </c>
     </row>
     <row r="6" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="E10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.35">
@@ -753,14 +753,14 @@
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>

</xml_diff>